<commit_message>
prueba hoja prediccion ingredientes
</commit_message>
<xml_diff>
--- a/ingredientes2016.xlsx
+++ b/ingredientes2016.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Reporte" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pizzas a la semana" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -134,860 +134,6 @@
     </indexedColors>
   </colors>
 </styleSheet>
-</file>
-
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <style val="5"/>
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>Pizzas pedidas</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <barChart>
-        <barDir val="col"/>
-        <grouping val="clustered"/>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <strRef>
-              <f>'Reporte'!B5</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'Reporte'!$A$6:$A$58</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Reporte'!$B$6:$B$58</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="1"/>
-          <order val="1"/>
-          <tx>
-            <strRef>
-              <f>'Reporte'!C5</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'Reporte'!$A$6:$A$58</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Reporte'!$C$6:$C$58</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="2"/>
-          <order val="2"/>
-          <tx>
-            <strRef>
-              <f>'Reporte'!D5</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'Reporte'!$A$6:$A$58</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Reporte'!$D$6:$D$58</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="3"/>
-          <order val="3"/>
-          <tx>
-            <strRef>
-              <f>'Reporte'!E5</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'Reporte'!$A$6:$A$58</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Reporte'!$E$6:$E$58</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="4"/>
-          <order val="4"/>
-          <tx>
-            <strRef>
-              <f>'Reporte'!F5</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'Reporte'!$A$6:$A$58</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Reporte'!$F$6:$F$58</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="5"/>
-          <order val="5"/>
-          <tx>
-            <strRef>
-              <f>'Reporte'!G5</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'Reporte'!$A$6:$A$58</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Reporte'!$G$6:$G$58</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="6"/>
-          <order val="6"/>
-          <tx>
-            <strRef>
-              <f>'Reporte'!H5</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'Reporte'!$A$6:$A$58</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Reporte'!$H$6:$H$58</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="7"/>
-          <order val="7"/>
-          <tx>
-            <strRef>
-              <f>'Reporte'!I5</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'Reporte'!$A$6:$A$58</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Reporte'!$I$6:$I$58</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="8"/>
-          <order val="8"/>
-          <tx>
-            <strRef>
-              <f>'Reporte'!J5</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'Reporte'!$A$6:$A$58</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Reporte'!$J$6:$J$58</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="9"/>
-          <order val="9"/>
-          <tx>
-            <strRef>
-              <f>'Reporte'!K5</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'Reporte'!$A$6:$A$58</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Reporte'!$K$6:$K$58</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="10"/>
-          <order val="10"/>
-          <tx>
-            <strRef>
-              <f>'Reporte'!L5</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'Reporte'!$A$6:$A$58</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Reporte'!$L$6:$L$58</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="11"/>
-          <order val="11"/>
-          <tx>
-            <strRef>
-              <f>'Reporte'!M5</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'Reporte'!$A$6:$A$58</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Reporte'!$M$6:$M$58</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="12"/>
-          <order val="12"/>
-          <tx>
-            <strRef>
-              <f>'Reporte'!N5</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'Reporte'!$A$6:$A$58</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Reporte'!$N$6:$N$58</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="13"/>
-          <order val="13"/>
-          <tx>
-            <strRef>
-              <f>'Reporte'!O5</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'Reporte'!$A$6:$A$58</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Reporte'!$O$6:$O$58</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="14"/>
-          <order val="14"/>
-          <tx>
-            <strRef>
-              <f>'Reporte'!P5</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'Reporte'!$A$6:$A$58</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Reporte'!$P$6:$P$58</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="15"/>
-          <order val="15"/>
-          <tx>
-            <strRef>
-              <f>'Reporte'!Q5</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'Reporte'!$A$6:$A$58</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Reporte'!$Q$6:$Q$58</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="16"/>
-          <order val="16"/>
-          <tx>
-            <strRef>
-              <f>'Reporte'!R5</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'Reporte'!$A$6:$A$58</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Reporte'!$R$6:$R$58</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="17"/>
-          <order val="17"/>
-          <tx>
-            <strRef>
-              <f>'Reporte'!S5</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'Reporte'!$A$6:$A$58</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Reporte'!$S$6:$S$58</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="18"/>
-          <order val="18"/>
-          <tx>
-            <strRef>
-              <f>'Reporte'!T5</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'Reporte'!$A$6:$A$58</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Reporte'!$T$6:$T$58</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="19"/>
-          <order val="19"/>
-          <tx>
-            <strRef>
-              <f>'Reporte'!U5</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'Reporte'!$A$6:$A$58</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Reporte'!$U$6:$U$58</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="20"/>
-          <order val="20"/>
-          <tx>
-            <strRef>
-              <f>'Reporte'!V5</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'Reporte'!$A$6:$A$58</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Reporte'!$V$6:$V$58</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="21"/>
-          <order val="21"/>
-          <tx>
-            <strRef>
-              <f>'Reporte'!W5</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'Reporte'!$A$6:$A$58</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Reporte'!$W$6:$W$58</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="22"/>
-          <order val="22"/>
-          <tx>
-            <strRef>
-              <f>'Reporte'!X5</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'Reporte'!$A$6:$A$58</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Reporte'!$X$6:$X$58</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="23"/>
-          <order val="23"/>
-          <tx>
-            <strRef>
-              <f>'Reporte'!Y5</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'Reporte'!$A$6:$A$58</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Reporte'!$Y$6:$Y$58</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="24"/>
-          <order val="24"/>
-          <tx>
-            <strRef>
-              <f>'Reporte'!Z5</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'Reporte'!$A$6:$A$58</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Reporte'!$Z$6:$Z$58</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="25"/>
-          <order val="25"/>
-          <tx>
-            <strRef>
-              <f>'Reporte'!AA5</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'Reporte'!$A$6:$A$58</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Reporte'!$AA$6:$AA$58</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="26"/>
-          <order val="26"/>
-          <tx>
-            <strRef>
-              <f>'Reporte'!AB5</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'Reporte'!$A$6:$A$58</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Reporte'!$AB$6:$AB$58</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="27"/>
-          <order val="27"/>
-          <tx>
-            <strRef>
-              <f>'Reporte'!AC5</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'Reporte'!$A$6:$A$58</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Reporte'!$AC$6:$AC$58</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="28"/>
-          <order val="28"/>
-          <tx>
-            <strRef>
-              <f>'Reporte'!AD5</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'Reporte'!$A$6:$A$58</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Reporte'!$AD$6:$AD$58</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="29"/>
-          <order val="29"/>
-          <tx>
-            <strRef>
-              <f>'Reporte'!AE5</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'Reporte'!$A$6:$A$58</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Reporte'!$AE$6:$AE$58</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="30"/>
-          <order val="30"/>
-          <tx>
-            <strRef>
-              <f>'Reporte'!AF5</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'Reporte'!$A$6:$A$58</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Reporte'!$AF$6:$AF$58</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="31"/>
-          <order val="31"/>
-          <tx>
-            <strRef>
-              <f>'Reporte'!AG5</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'Reporte'!$A$6:$A$58</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Reporte'!$AG$6:$AG$58</f>
-            </numRef>
-          </val>
-        </ser>
-        <gapWidth val="150"/>
-        <axId val="10"/>
-        <axId val="100"/>
-      </barChart>
-      <catAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="100"/>
-        <lblOffset val="100"/>
-      </catAx>
-      <valAx>
-        <axId val="100"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="r"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <oneCellAnchor>
-    <from>
-      <col>34</col>
-      <colOff>0</colOff>
-      <row>33</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="5400000" cy="2700000"/>
-    <graphicFrame>
-      <nvGraphicFramePr>
-        <cNvPr id="1" name="Chart 1"/>
-        <cNvGraphicFramePr/>
-      </nvGraphicFramePr>
-      <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </graphicFrame>
-    <clientData/>
-  </oneCellAnchor>
-</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6809,6 +5955,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>